<commit_message>
Edited some files because other groups are bad at taking data
</commit_message>
<xml_diff>
--- a/Exp 2 (airfoil) data files/AirfoilPressure_S2_2.xlsx
+++ b/Exp 2 (airfoil) data files/AirfoilPressure_S2_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/College Documents/Sophomore Year/Intro to Thermo:Aero/ASEN2002_Lab2/Exp 2 (airfoil) data files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCA505E4-711E-6F46-9BB1-93E3DCB45F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4D0735B7-8F81-F048-8AB3-CF32D1D58D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AirfoilPressure_S2_2" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -954,10 +954,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>